<commit_message>
Implementação da gestão de autenticações.
</commit_message>
<xml_diff>
--- a/docs/miguel costa base dados.xlsx
+++ b/docs/miguel costa base dados.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
     <sheet name="Folha2" sheetId="2" r:id="rId2"/>
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Fornecedores:</t>
   </si>
@@ -133,6 +138,51 @@
   </si>
   <si>
     <t>produto descrição</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Páginas</t>
+  </si>
+  <si>
+    <t>Fornecedores</t>
+  </si>
+  <si>
+    <t>Listar</t>
+  </si>
+  <si>
+    <t>Gerir</t>
+  </si>
+  <si>
+    <t>id do produto</t>
+  </si>
+  <si>
+    <t>Produtos</t>
+  </si>
+  <si>
+    <t>Ajustar quantidade</t>
+  </si>
+  <si>
+    <t>Obras</t>
+  </si>
+  <si>
+    <t>f10</t>
+  </si>
+  <si>
+    <t>Dentro de uma obra</t>
+  </si>
+  <si>
+    <t>Dá para adicionar produtos e gerir quantidades/preços</t>
+  </si>
+  <si>
+    <t>Logins</t>
+  </si>
+  <si>
+    <t>Utilizadores</t>
+  </si>
+  <si>
+    <t>http://norconcept.pt/</t>
   </si>
 </sst>
 </file>
@@ -480,26 +530,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -524,13 +577,48 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="P3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="Q4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="P5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="Q7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -555,24 +643,48 @@
       <c r="M8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="I9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="I10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="P10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="E11" t="s">
         <v>13</v>
       </c>
@@ -580,7 +692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19">
       <c r="E12" t="s">
         <v>14</v>
       </c>
@@ -588,7 +700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19">
       <c r="E13" t="s">
         <v>15</v>
       </c>
@@ -596,12 +708,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19">
       <c r="I14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -630,12 +745,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14">
       <c r="B21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14">
       <c r="B23" t="s">
         <v>36</v>
       </c>
@@ -661,9 +776,22 @@
         <v>28</v>
       </c>
     </row>
+    <row r="24" spans="1:14">
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -673,9 +801,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -685,8 +818,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>